<commit_message>
Merge k Sorted Lists
</commit_message>
<xml_diff>
--- a/WorkBook.xlsx
+++ b/WorkBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93A45C2-D849-4FF6-8597-F46CAEB0F723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2C7598-33A1-4CD6-A61E-AF9ABA5C4F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FC43D204-5A26-453C-8339-0FD2D18C7DE7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>PROBLEM NUMBER</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>Merge k Sorted Lists</t>
+  </si>
+  <si>
+    <t>HARD</t>
   </si>
 </sst>
 </file>
@@ -423,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8A7844-C39B-440D-874C-A4F00DB0DADA}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +480,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated workbook with more tree problems
</commit_message>
<xml_diff>
--- a/WorkBook.xlsx
+++ b/WorkBook.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>DATE</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Binary Tree Inorder Traversal</t>
+  </si>
+  <si>
+    <t>Same tree</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -597,12 +603,24 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="4">
+        <v>44360.0</v>
+      </c>
+      <c r="B7" s="5">
+        <v>100.0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -625,12 +643,24 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="4">
+        <v>44360.0</v>
+      </c>
+      <c r="B8" s="5">
+        <v>110.0</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>

</xml_diff>